<commit_message>
updated to Python 3.10 and added NLLB-200
</commit_message>
<xml_diff>
--- a/domain_specific_machine_translation/v_evaluation/results.xlsx
+++ b/domain_specific_machine_translation/v_evaluation/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.256</v>
+        <v>0.249</v>
       </c>
       <c r="C2" t="n">
-        <v>0.433</v>
+        <v>0.421</v>
       </c>
       <c r="D2" t="n">
-        <v>0.597</v>
+        <v>0.596</v>
       </c>
     </row>
     <row r="3">
@@ -473,45 +473,77 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.388</v>
+        <v>0.379</v>
       </c>
       <c r="C3" t="n">
-        <v>0.552</v>
+        <v>0.541</v>
       </c>
       <c r="D3" t="n">
-        <v>0.717</v>
+        <v>0.709</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>t5-base</t>
+          <t>t5-large</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.166</v>
+        <v>0.173</v>
       </c>
       <c r="C4" t="n">
-        <v>0.307</v>
+        <v>0.297</v>
       </c>
       <c r="D4" t="n">
-        <v>0.309</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>t5-base_finetuned</t>
+          <t>t5-large_finetuned</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.34</v>
+        <v>0.367</v>
       </c>
       <c r="C5" t="n">
-        <v>0.492</v>
+        <v>0.521</v>
       </c>
       <c r="D5" t="n">
-        <v>0.662</v>
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>facebook/nllb-200-distilled-600M</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.411</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.595</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>facebook/nllb-200-distilled-600M_finetuned</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.531</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>